<commit_message>
added paml results for mito
</commit_message>
<xml_diff>
--- a/mauve_alignments/cat_alignments/codeml/LRTs.xlsx
+++ b/mauve_alignments/cat_alignments/codeml/LRTs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maeperez/Desktop/VesicSymb_Evolution/mauve_alignments/cat_alignments/codeml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F60190-8F96-CE48-9E81-20AD8975C0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A181D8-AE0A-0547-A81E-4963E4EAAECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2480" windowWidth="26740" windowHeight="14420" activeTab="1" xr2:uid="{7BDD606C-C06A-C643-8E24-BADE6ACAE95F}"/>
   </bookViews>
@@ -35,10 +35,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
+  <si>
+    <t>Wfl = W2 = wb = w1</t>
+  </si>
+  <si>
+    <t>wfl != w2 != wb = w1</t>
+  </si>
+  <si>
+    <t>wfl != w2 = wb = w1</t>
+  </si>
+  <si>
+    <t>wfl != w2 = w1 != wb</t>
+  </si>
+  <si>
+    <t>H2: Long term shift in selection on both Clade I and Clade II; those lineages are subject to selection pressures different from each other and from the ancestor.</t>
+  </si>
+  <si>
+    <t>H1: Long term shift in selection on in the symbionts. Clade I and II have the same selective pressure</t>
+  </si>
+  <si>
+    <t>LNL</t>
+  </si>
+  <si>
+    <t>pval</t>
+  </si>
+  <si>
+    <t>H3: Episodic change in selection pressure in the the branch leading to Clade I (branch b ).</t>
+  </si>
+  <si>
+    <t>H0</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>np 
+(number of parameters)</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>wfl != w2 != w1 != wb</t>
+  </si>
+  <si>
+    <t>wfl != w2 != w1 = wb</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>&lt;.00001</t>
+  </si>
   <si>
     <r>
-      <t>H0: homogeneous selection pressure over the tree; rate increase in </t>
+      <t>H0: Homogeneous selection pressure over the tree; (rate increase in </t>
     </r>
     <r>
       <rPr>
@@ -57,76 +115,49 @@
         <rFont val="Helvetica Neue"/>
         <family val="2"/>
       </rPr>
-      <t> is simply due to an underlying increase in the mutation rate;</t>
+      <t> is simply due to an underlying increase in the mutation rate;)</t>
     </r>
   </si>
   <si>
-    <t>Wfl = W2 = wb = w1</t>
-  </si>
-  <si>
-    <t>wfl != w2 != wb = w1</t>
-  </si>
-  <si>
-    <t>wfl != w2 = wb = w1</t>
-  </si>
-  <si>
-    <t>wfl != w2 = w1 != wb</t>
-  </si>
-  <si>
-    <t>H2: Long term shift in selection on both Clade I and Clade II; those lineages are subject to selection pressures different from each other and from the ancestor.</t>
-  </si>
-  <si>
-    <t>H1: Long term shift in selection on in the symbionts. Clade I and II have the same selective pressure</t>
-  </si>
-  <si>
-    <t>LNL</t>
-  </si>
-  <si>
-    <t>pval</t>
-  </si>
-  <si>
-    <t>H3: Episodic change in selection pressure in the the branch leading to Clade I (branch b ).</t>
-  </si>
-  <si>
-    <t>codeml - MITO</t>
-  </si>
-  <si>
-    <t>H0</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>np 
-(number of parameters)</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>wfl != w2 != w1 != wb</t>
-  </si>
-  <si>
-    <t>wfl != w2 != w1 = wb</t>
-  </si>
-  <si>
-    <t>H4</t>
-  </si>
-  <si>
-    <t>H4:</t>
+    <t>H0: Homogeneous mutation rate over the tree</t>
+  </si>
+  <si>
+    <t>H1: Homogeneous mutation rate amongst the Vesicomyid; Bathy is the outgroup</t>
+  </si>
+  <si>
+    <t>H3: Shift in substition rate on the diverging Clade I branch only; Clade I and Clade II have the same substitution rate</t>
+  </si>
+  <si>
+    <t>H4: Shift in substition rate on the diverging Clade I and branch b and Clade II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clade I substitution != Clade II substitution </t>
+  </si>
+  <si>
+    <t>Clade I substitution = branch b substitution</t>
+  </si>
+  <si>
+    <t>codeml - MITO; significant differences between dnds on Bathy and on Vesic species, not amongst Vesic clades</t>
+  </si>
+  <si>
+    <t>H2: Shift in substitution rate between Clade I, Clade II and Bathy</t>
+  </si>
+  <si>
+    <t>codeml - MITO; significant substitution change in rate between Bathy, Clade I and Clade II overall but not between branch b and Clade I or between Clade I (branch b excluded) and Clade II.
+Inequal triangle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codeml - SYMB; </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,14 +184,33 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -328,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -336,16 +386,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -382,12 +441,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -401,6 +454,36 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,178 +801,181 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="52.1640625" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="138.83203125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="14" customWidth="1"/>
-    <col min="3" max="5" width="9" style="14" customWidth="1"/>
-    <col min="6" max="10" width="10.5" style="14" customWidth="1"/>
-    <col min="11" max="16384" width="52.1640625" style="14"/>
+    <col min="1" max="1" width="138.83203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="17" customWidth="1"/>
+    <col min="3" max="5" width="9" style="17" customWidth="1"/>
+    <col min="6" max="10" width="10.5" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="52.1640625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="I1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17">
+        <v>-50845.811249999999</v>
+      </c>
+      <c r="D2" s="17">
+        <v>36</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="17">
+        <v>-50840.102422000004</v>
+      </c>
+      <c r="D3" s="17">
+        <v>37</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="32">
+        <v>7.2800000000000002E-4</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="17">
+        <v>-50840.540372000003</v>
+      </c>
+      <c r="D4" s="17">
+        <v>38</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="32">
+        <v>5.1409999999999997E-3</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0.15729899999999999</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="21"/>
+    </row>
+    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="17">
+        <v>-50841.184262000002</v>
+      </c>
+      <c r="D5" s="17">
+        <v>38</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="32">
+        <v>9.7850000000000003E-3</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0.14131299999999999</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="14">
-        <v>-50845.811249999999</v>
-      </c>
-      <c r="D2" s="14">
-        <v>36</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="14">
-        <v>-50840.102422000004</v>
-      </c>
-      <c r="D3" s="14">
-        <v>37</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="17">
-        <v>7.2800000000000002E-4</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
-        <v>-50840.540372000003</v>
-      </c>
-      <c r="D4" s="14">
-        <v>38</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="17">
-        <v>5.1409999999999997E-3</v>
-      </c>
-      <c r="H4" s="17">
-        <v>0.15729899999999999</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="14">
-        <v>-50841.184262000002</v>
-      </c>
-      <c r="D5" s="14">
-        <v>38</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="17">
-        <v>9.7850000000000003E-3</v>
-      </c>
-      <c r="H5" s="17">
-        <v>0.14131299999999999</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="17">
+        <v>-50839.916811000003</v>
+      </c>
+      <c r="D6" s="17">
+        <v>39</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="14">
-        <v>-50839.916811000003</v>
-      </c>
-      <c r="D6" s="14">
-        <v>39</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="19">
+      <c r="G6" s="33">
         <v>8.1460000000000005E-3</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="31">
         <v>0.83060599999999996</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="31">
         <v>0.115949</v>
       </c>
-      <c r="J6" s="20">
-        <v>1.111354</v>
+      <c r="J6" s="34">
+        <v>0.11135399999999999</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F8" s="14">
+      <c r="F8" s="17">
         <f>2*ABS(C6-C2)</f>
         <v>11.78887799999211</v>
       </c>
@@ -908,151 +994,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E022A0B-EAC7-0541-80DE-77E3FA00C411}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="99" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" customWidth="1"/>
-    <col min="6" max="10" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="10" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
+    <row r="1" spans="1:11" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>28</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" s="2"/>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="J1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>14</v>
-      </c>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-57073.422792999998</v>
+      <c r="C2" s="26">
+        <v>-57066.277619</v>
       </c>
       <c r="D2" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3"/>
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1.5699999999999999E-4</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>6</v>
+      <c r="A3" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="26">
+        <v>-57073.422792999998</v>
+      </c>
+      <c r="D3" s="1">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-57055.492598999997</v>
+      </c>
+      <c r="D4" s="1">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="25">
-        <v>-57073.422792999998</v>
-      </c>
-      <c r="D3" s="1">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-55718.031496000003</v>
-      </c>
-      <c r="D4" s="1">
-        <v>193</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" s="1">
-        <v>-55718.029628999997</v>
+        <v>-57055.492598999997</v>
       </c>
       <c r="D5" s="1">
-        <v>193</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="6"/>
+      <c r="F5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="6">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="28">
+        <v>1</v>
+      </c>
+      <c r="J5" s="29">
+        <v>1</v>
+      </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>-55718.029628999997</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>-57055.492598999997</v>
+      </c>
+      <c r="D6" s="1">
+        <v>26</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1068,18 +1182,191 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="27">
+        <f>2*ABS(C4-C3)</f>
+        <v>35.860388000000967</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="38" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="27">
+        <f>2*ABS(C4-C2)</f>
+        <v>21.570040000005974</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="38" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="27">
+        <f>2*ABS(C6-C3)</f>
+        <v>35.860388000000967</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="1:11" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" ht="96" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="27">
+        <f>2*ABS(C15-C14)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="27">
+        <f>2*ABS(C15-C13)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+      <c r="G20" s="27">
+        <f>2*ABS(C17-C14)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>